<commit_message>
Ultimas funciones auxiliares Lectura Datos
</commit_message>
<xml_diff>
--- a/inst/extdata/tablas_finales_2.xlsx
+++ b/inst/extdata/tablas_finales_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9e6fb069572b4b3/Escritorio/TFG ESTADISTICA/paquete.elecciones/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacho\OneDrive\Escritorio\TFG ESTADISTICA\paquete.elecciones\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_428A0E65050AEB533E85682CE43F697BED03D505" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD5BB695-DFD6-4A90-9D46-189DCDF9415B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E7B033-3D59-44A6-9C79-5FEB8D616D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="13520" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="13520" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01xxaamm.DAT" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="220">
   <si>
     <t>Inicio</t>
   </si>
@@ -321,9 +321,6 @@
     <t>número_vuelta</t>
   </si>
   <si>
-    <t>codigo_provincia_INE</t>
-  </si>
-  <si>
     <t>distrito_electoral</t>
   </si>
   <si>
@@ -622,9 +619,6 @@
   </si>
   <si>
     <t>Censo de escrutinio o censo C.E.R.A.</t>
-  </si>
-  <si>
-    <t>codigo_provincia_cera</t>
   </si>
   <si>
     <t>codigo_seccion</t>
@@ -1539,7 +1533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
@@ -1565,42 +1561,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
@@ -1620,7 +1616,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
@@ -1697,10 +1693,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
@@ -1717,10 +1713,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F9" t="s">
-        <v>197</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
@@ -1737,10 +1733,10 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
@@ -1757,10 +1753,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -1777,10 +1773,10 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
@@ -1797,10 +1793,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
@@ -1817,10 +1813,10 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
@@ -1837,10 +1833,10 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F15" t="s">
         <v>205</v>
-      </c>
-      <c r="F15" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1878,42 +1874,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
@@ -1930,10 +1926,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
@@ -2010,10 +2006,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
@@ -2030,10 +2026,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
@@ -2050,10 +2046,10 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
@@ -2070,10 +2066,10 @@
         <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -2090,10 +2086,10 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
@@ -2110,10 +2106,10 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
@@ -2130,10 +2126,10 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
@@ -2150,10 +2146,10 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
@@ -2170,10 +2166,10 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
@@ -2190,10 +2186,10 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
@@ -2210,10 +2206,10 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
@@ -2230,10 +2226,10 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
@@ -2250,10 +2246,10 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
@@ -2270,10 +2266,10 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
@@ -2290,10 +2286,10 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.5">
@@ -2310,10 +2306,10 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.5">
@@ -2330,10 +2326,10 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
@@ -2350,10 +2346,10 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.5">
@@ -2370,10 +2366,10 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F26" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.5">
@@ -2390,10 +2386,10 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2405,7 +2401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
@@ -2431,42 +2427,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
@@ -2483,10 +2479,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
@@ -2563,10 +2559,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
@@ -2583,10 +2579,10 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
@@ -2623,10 +2619,10 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -2643,10 +2639,10 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
@@ -2666,7 +2662,7 @@
         <v>85</v>
       </c>
       <c r="F13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
@@ -2686,7 +2682,7 @@
         <v>86</v>
       </c>
       <c r="F14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
@@ -2706,7 +2702,7 @@
         <v>87</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
@@ -2726,7 +2722,7 @@
         <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
@@ -2746,7 +2742,7 @@
         <v>89</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
@@ -2766,7 +2762,7 @@
         <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
@@ -2786,7 +2782,7 @@
         <v>91</v>
       </c>
       <c r="F19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
@@ -2803,10 +2799,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
@@ -2823,10 +2819,10 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
+        <v>217</v>
+      </c>
+      <c r="F21" t="s">
         <v>219</v>
-      </c>
-      <c r="F21" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
@@ -2846,7 +2842,7 @@
         <v>93</v>
       </c>
       <c r="F22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3448,7 +3444,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
@@ -3609,7 +3607,7 @@
         <v>80</v>
       </c>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
@@ -3629,7 +3627,7 @@
         <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
@@ -3649,7 +3647,7 @@
         <v>82</v>
       </c>
       <c r="F10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
@@ -3689,7 +3687,7 @@
         <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
@@ -3709,7 +3707,7 @@
         <v>84</v>
       </c>
       <c r="F13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
@@ -3729,7 +3727,7 @@
         <v>85</v>
       </c>
       <c r="F14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
@@ -3749,7 +3747,7 @@
         <v>86</v>
       </c>
       <c r="F15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
@@ -3769,7 +3767,7 @@
         <v>87</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
@@ -3789,7 +3787,7 @@
         <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
@@ -3809,7 +3807,7 @@
         <v>89</v>
       </c>
       <c r="F18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
@@ -3829,7 +3827,7 @@
         <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
@@ -3849,7 +3847,7 @@
         <v>91</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
@@ -3869,7 +3867,7 @@
         <v>92</v>
       </c>
       <c r="F21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
@@ -3889,7 +3887,7 @@
         <v>93</v>
       </c>
       <c r="F22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3901,8 +3899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3932,42 +3930,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
@@ -4044,10 +4042,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
@@ -4064,10 +4062,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
@@ -4084,10 +4082,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
@@ -4104,10 +4102,10 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
@@ -4124,10 +4122,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -4144,10 +4142,10 @@
         <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
@@ -4164,10 +4162,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
@@ -4184,10 +4182,10 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
@@ -4204,10 +4202,10 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
@@ -4224,10 +4222,10 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
@@ -4244,10 +4242,10 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
@@ -4264,10 +4262,10 @@
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
@@ -4284,10 +4282,10 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
@@ -4304,10 +4302,10 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
@@ -4324,10 +4322,10 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
@@ -4344,10 +4342,10 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.5">
@@ -4364,10 +4362,10 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.5">
@@ -4384,10 +4382,10 @@
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
@@ -4404,10 +4402,10 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.5">
@@ -4424,10 +4422,10 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.5">
@@ -4444,10 +4442,10 @@
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.5">
@@ -4464,10 +4462,10 @@
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.5">
@@ -4484,10 +4482,10 @@
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.5">
@@ -4504,10 +4502,10 @@
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.5">
@@ -4524,10 +4522,10 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4539,7 +4537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
@@ -4565,42 +4563,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
@@ -4620,7 +4618,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
@@ -4697,10 +4695,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
@@ -4717,10 +4715,10 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
@@ -4737,10 +4735,10 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
@@ -4757,10 +4755,10 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -4777,10 +4775,10 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
@@ -4797,10 +4795,10 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -4812,7 +4810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
@@ -4838,42 +4838,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
@@ -4893,7 +4893,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
@@ -4950,10 +4950,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
@@ -4970,10 +4970,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
@@ -4990,10 +4990,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F9" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
@@ -5010,10 +5010,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
@@ -5030,10 +5030,10 @@
         <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -5050,10 +5050,10 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
@@ -5070,10 +5070,10 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
@@ -5090,10 +5090,10 @@
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
@@ -5110,10 +5110,10 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
@@ -5130,10 +5130,10 @@
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
@@ -5150,10 +5150,10 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
@@ -5170,10 +5170,10 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
@@ -5190,10 +5190,10 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
@@ -5210,10 +5210,10 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
@@ -5230,10 +5230,10 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
@@ -5250,10 +5250,10 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.5">
@@ -5270,10 +5270,10 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.5">
@@ -5290,10 +5290,10 @@
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
@@ -5310,10 +5310,10 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.5">
@@ -5330,10 +5330,10 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -5345,7 +5345,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
@@ -5371,42 +5373,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
@@ -5503,10 +5505,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
@@ -5523,10 +5525,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F9" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
@@ -5543,10 +5545,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
@@ -5563,10 +5565,10 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -5583,10 +5585,10 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
@@ -5603,10 +5605,10 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -5618,9 +5620,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="5" max="5" width="209.76171875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
@@ -5644,42 +5651,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
@@ -5756,10 +5763,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
@@ -5776,10 +5783,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
@@ -5796,10 +5803,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F9" t="s">
-        <v>197</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
@@ -5816,10 +5823,10 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
@@ -5836,10 +5843,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -5856,10 +5863,10 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
@@ -5876,10 +5883,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
@@ -5896,10 +5903,10 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
@@ -5916,10 +5923,10 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
@@ -5936,10 +5943,10 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
@@ -5956,10 +5963,10 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
@@ -5976,10 +5983,10 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
@@ -5996,10 +6003,10 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
@@ -6016,10 +6023,10 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
@@ -6036,10 +6043,10 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
@@ -6056,10 +6063,10 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.5">
@@ -6076,10 +6083,10 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.5">
@@ -6096,10 +6103,10 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
@@ -6116,10 +6123,10 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>